<commit_message>
added more cars to the specs file
</commit_message>
<xml_diff>
--- a/Specs.xlsx
+++ b/Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gduncan\Downloads\vroom_vroom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14A3A01-A24D-4827-9248-FF2AEDD3775A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F37FC1-ADA8-4182-ABFC-32CF344E4FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A311B30-B3A1-4A32-B3E5-E04E58484C82}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="76">
   <si>
     <t>Make</t>
   </si>
@@ -165,6 +165,105 @@
   </si>
   <si>
     <t>C:\Users\gduncan\Downloads\vroom_vroom\images\Pilot.jpg</t>
+  </si>
+  <si>
+    <t>Nissan</t>
+  </si>
+  <si>
+    <t>Maxima</t>
+  </si>
+  <si>
+    <t>Acura</t>
+  </si>
+  <si>
+    <t>MDX</t>
+  </si>
+  <si>
+    <t>Chevrolet</t>
+  </si>
+  <si>
+    <t>Suburban</t>
+  </si>
+  <si>
+    <t>Tahoe</t>
+  </si>
+  <si>
+    <t>Dodge</t>
+  </si>
+  <si>
+    <t>Charger</t>
+  </si>
+  <si>
+    <t>GMC</t>
+  </si>
+  <si>
+    <t>Yukon</t>
+  </si>
+  <si>
+    <t>Odyssey</t>
+  </si>
+  <si>
+    <t>Hyundai</t>
+  </si>
+  <si>
+    <t>Palisade</t>
+  </si>
+  <si>
+    <t>Jeep</t>
+  </si>
+  <si>
+    <t>Cherokee</t>
+  </si>
+  <si>
+    <t>Wagoneer</t>
+  </si>
+  <si>
+    <t>Wrangler</t>
+  </si>
+  <si>
+    <t>Kia</t>
+  </si>
+  <si>
+    <t>EV6</t>
+  </si>
+  <si>
+    <t>Lincoln</t>
+  </si>
+  <si>
+    <t>Aviator</t>
+  </si>
+  <si>
+    <t>Subaru</t>
+  </si>
+  <si>
+    <t>Ascent</t>
+  </si>
+  <si>
+    <t>Forester</t>
+  </si>
+  <si>
+    <t>Model 3</t>
+  </si>
+  <si>
+    <t>Model S</t>
+  </si>
+  <si>
+    <t>Model X</t>
+  </si>
+  <si>
+    <t>RAV4</t>
+  </si>
+  <si>
+    <t>Sequoia</t>
+  </si>
+  <si>
+    <t>Volkswagen</t>
+  </si>
+  <si>
+    <t>Atlas</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -517,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB2CE35-0282-4446-A502-23F50F608244}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -533,7 +632,7 @@
     <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.109375" bestFit="1" customWidth="1"/>
@@ -964,6 +1063,930 @@
         <v>40</v>
       </c>
     </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10">
+        <v>2023</v>
+      </c>
+      <c r="E10">
+        <v>45</v>
+      </c>
+      <c r="F10">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="G10">
+        <v>24</v>
+      </c>
+      <c r="H10">
+        <v>30</v>
+      </c>
+      <c r="I10">
+        <v>20</v>
+      </c>
+      <c r="J10" s="1">
+        <v>43300</v>
+      </c>
+      <c r="K10" t="s">
+        <v>29</v>
+      </c>
+      <c r="L10">
+        <v>6</v>
+      </c>
+      <c r="M10" t="s">
+        <v>26</v>
+      </c>
+      <c r="N10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11">
+        <v>2022</v>
+      </c>
+      <c r="E11">
+        <v>41.6</v>
+      </c>
+      <c r="F11">
+        <v>38.5</v>
+      </c>
+      <c r="G11">
+        <v>21</v>
+      </c>
+      <c r="H11">
+        <v>25</v>
+      </c>
+      <c r="I11">
+        <v>19</v>
+      </c>
+      <c r="J11" s="1">
+        <v>54900</v>
+      </c>
+      <c r="K11" t="s">
+        <v>29</v>
+      </c>
+      <c r="L11">
+        <v>6</v>
+      </c>
+      <c r="M11" t="s">
+        <v>26</v>
+      </c>
+      <c r="N11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12">
+        <v>2022</v>
+      </c>
+      <c r="E12">
+        <v>44.5</v>
+      </c>
+      <c r="F12">
+        <v>42</v>
+      </c>
+      <c r="G12">
+        <v>17</v>
+      </c>
+      <c r="H12">
+        <v>20</v>
+      </c>
+      <c r="I12">
+        <v>15</v>
+      </c>
+      <c r="J12" s="1">
+        <v>57800</v>
+      </c>
+      <c r="K12" t="s">
+        <v>29</v>
+      </c>
+      <c r="L12">
+        <v>8</v>
+      </c>
+      <c r="M12" t="s">
+        <v>26</v>
+      </c>
+      <c r="N12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13">
+        <v>2022</v>
+      </c>
+      <c r="E13">
+        <v>44.5</v>
+      </c>
+      <c r="F13">
+        <v>42</v>
+      </c>
+      <c r="G13">
+        <v>17</v>
+      </c>
+      <c r="H13">
+        <v>20</v>
+      </c>
+      <c r="I13">
+        <v>15</v>
+      </c>
+      <c r="J13" s="1">
+        <v>58100</v>
+      </c>
+      <c r="K13" t="s">
+        <v>29</v>
+      </c>
+      <c r="L13">
+        <v>8</v>
+      </c>
+      <c r="M13" t="s">
+        <v>26</v>
+      </c>
+      <c r="N13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14">
+        <v>2022</v>
+      </c>
+      <c r="E14">
+        <v>41.8</v>
+      </c>
+      <c r="F14">
+        <v>40.1</v>
+      </c>
+      <c r="G14">
+        <v>21</v>
+      </c>
+      <c r="H14">
+        <v>27</v>
+      </c>
+      <c r="I14">
+        <v>18</v>
+      </c>
+      <c r="J14" s="1">
+        <v>38275</v>
+      </c>
+      <c r="K14" t="s">
+        <v>29</v>
+      </c>
+      <c r="L14">
+        <v>6</v>
+      </c>
+      <c r="M14" t="s">
+        <v>26</v>
+      </c>
+      <c r="N14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15">
+        <v>2022</v>
+      </c>
+      <c r="E15">
+        <v>42</v>
+      </c>
+      <c r="F15">
+        <v>44.5</v>
+      </c>
+      <c r="G15">
+        <v>17</v>
+      </c>
+      <c r="H15">
+        <v>20</v>
+      </c>
+      <c r="I15">
+        <v>15</v>
+      </c>
+      <c r="J15" s="1">
+        <v>54600</v>
+      </c>
+      <c r="K15" t="s">
+        <v>29</v>
+      </c>
+      <c r="L15">
+        <v>8</v>
+      </c>
+      <c r="M15" t="s">
+        <v>26</v>
+      </c>
+      <c r="N15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16">
+        <v>2022</v>
+      </c>
+      <c r="E16">
+        <v>40.9</v>
+      </c>
+      <c r="F16">
+        <v>40.9</v>
+      </c>
+      <c r="G16">
+        <v>22</v>
+      </c>
+      <c r="H16">
+        <v>28</v>
+      </c>
+      <c r="I16">
+        <v>19</v>
+      </c>
+      <c r="J16" s="1">
+        <v>48770</v>
+      </c>
+      <c r="K16" t="s">
+        <v>29</v>
+      </c>
+      <c r="L16">
+        <v>6</v>
+      </c>
+      <c r="M16" t="s">
+        <v>28</v>
+      </c>
+      <c r="N16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17">
+        <v>2022</v>
+      </c>
+      <c r="E17">
+        <v>44.1</v>
+      </c>
+      <c r="F17">
+        <v>42.4</v>
+      </c>
+      <c r="G17">
+        <v>21</v>
+      </c>
+      <c r="H17">
+        <v>24</v>
+      </c>
+      <c r="I17">
+        <v>19</v>
+      </c>
+      <c r="J17" s="1">
+        <v>35300</v>
+      </c>
+      <c r="K17" t="s">
+        <v>29</v>
+      </c>
+      <c r="L17">
+        <v>6</v>
+      </c>
+      <c r="M17" t="s">
+        <v>26</v>
+      </c>
+      <c r="N17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18">
+        <v>2022</v>
+      </c>
+      <c r="E18">
+        <v>41.3</v>
+      </c>
+      <c r="F18">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="G18">
+        <v>22</v>
+      </c>
+      <c r="H18">
+        <v>26</v>
+      </c>
+      <c r="I18">
+        <v>19</v>
+      </c>
+      <c r="J18" s="1">
+        <v>46645</v>
+      </c>
+      <c r="K18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L18">
+        <v>6</v>
+      </c>
+      <c r="M18" t="s">
+        <v>26</v>
+      </c>
+      <c r="N18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19">
+        <v>2022</v>
+      </c>
+      <c r="E19">
+        <v>40.9</v>
+      </c>
+      <c r="F19">
+        <v>42.7</v>
+      </c>
+      <c r="G19">
+        <v>18</v>
+      </c>
+      <c r="H19">
+        <v>22</v>
+      </c>
+      <c r="I19">
+        <v>16</v>
+      </c>
+      <c r="J19" s="1">
+        <v>68995</v>
+      </c>
+      <c r="K19" t="s">
+        <v>29</v>
+      </c>
+      <c r="L19">
+        <v>8</v>
+      </c>
+      <c r="M19" t="s">
+        <v>26</v>
+      </c>
+      <c r="N19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20">
+        <v>2022</v>
+      </c>
+      <c r="E20">
+        <v>41.2</v>
+      </c>
+      <c r="F20">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="G20">
+        <v>19</v>
+      </c>
+      <c r="H20">
+        <v>23</v>
+      </c>
+      <c r="I20">
+        <v>17</v>
+      </c>
+      <c r="J20" s="1">
+        <v>39240</v>
+      </c>
+      <c r="K20" t="s">
+        <v>29</v>
+      </c>
+      <c r="L20">
+        <v>6</v>
+      </c>
+      <c r="M20" t="s">
+        <v>26</v>
+      </c>
+      <c r="N20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21">
+        <v>2022</v>
+      </c>
+      <c r="E21">
+        <v>42.4</v>
+      </c>
+      <c r="F21">
+        <v>39</v>
+      </c>
+      <c r="G21">
+        <v>105</v>
+      </c>
+      <c r="H21">
+        <v>94</v>
+      </c>
+      <c r="I21">
+        <v>116</v>
+      </c>
+      <c r="J21" s="1">
+        <v>51400</v>
+      </c>
+      <c r="K21" t="s">
+        <v>24</v>
+      </c>
+      <c r="L21" t="s">
+        <v>24</v>
+      </c>
+      <c r="M21" t="s">
+        <v>26</v>
+      </c>
+      <c r="N21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22">
+        <v>2022</v>
+      </c>
+      <c r="E22">
+        <v>43</v>
+      </c>
+      <c r="F22">
+        <v>39</v>
+      </c>
+      <c r="G22">
+        <v>20</v>
+      </c>
+      <c r="H22">
+        <v>24</v>
+      </c>
+      <c r="I22">
+        <v>17</v>
+      </c>
+      <c r="J22" s="1">
+        <v>54285</v>
+      </c>
+      <c r="K22" t="s">
+        <v>29</v>
+      </c>
+      <c r="L22">
+        <v>6</v>
+      </c>
+      <c r="M22" t="s">
+        <v>26</v>
+      </c>
+      <c r="N22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23">
+        <v>2022</v>
+      </c>
+      <c r="E23">
+        <v>42.2</v>
+      </c>
+      <c r="F23">
+        <v>38.6</v>
+      </c>
+      <c r="G23">
+        <v>23</v>
+      </c>
+      <c r="H23">
+        <v>27</v>
+      </c>
+      <c r="I23">
+        <v>21</v>
+      </c>
+      <c r="J23" s="1">
+        <v>35295</v>
+      </c>
+      <c r="K23" t="s">
+        <v>29</v>
+      </c>
+      <c r="L23">
+        <v>4</v>
+      </c>
+      <c r="M23" t="s">
+        <v>26</v>
+      </c>
+      <c r="N23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24">
+        <v>2022</v>
+      </c>
+      <c r="E24">
+        <v>43.3</v>
+      </c>
+      <c r="F24">
+        <v>39.4</v>
+      </c>
+      <c r="G24">
+        <v>29</v>
+      </c>
+      <c r="H24">
+        <v>33</v>
+      </c>
+      <c r="I24">
+        <v>26</v>
+      </c>
+      <c r="J24" s="1">
+        <v>32575</v>
+      </c>
+      <c r="K24" t="s">
+        <v>29</v>
+      </c>
+      <c r="L24">
+        <v>4</v>
+      </c>
+      <c r="M24" t="s">
+        <v>26</v>
+      </c>
+      <c r="N24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25">
+        <v>2022</v>
+      </c>
+      <c r="E25">
+        <v>42.7</v>
+      </c>
+      <c r="F25">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="G25">
+        <v>113</v>
+      </c>
+      <c r="H25">
+        <v>107</v>
+      </c>
+      <c r="I25">
+        <v>118</v>
+      </c>
+      <c r="J25" s="1">
+        <v>62990</v>
+      </c>
+      <c r="K25" t="s">
+        <v>24</v>
+      </c>
+      <c r="L25" t="s">
+        <v>24</v>
+      </c>
+      <c r="M25" t="s">
+        <v>26</v>
+      </c>
+      <c r="N25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26">
+        <v>2022</v>
+      </c>
+      <c r="E26">
+        <v>42.4</v>
+      </c>
+      <c r="F26">
+        <v>35.5</v>
+      </c>
+      <c r="G26">
+        <v>120</v>
+      </c>
+      <c r="H26">
+        <v>115</v>
+      </c>
+      <c r="I26">
+        <v>124</v>
+      </c>
+      <c r="J26" s="1">
+        <v>104990</v>
+      </c>
+      <c r="K26" t="s">
+        <v>24</v>
+      </c>
+      <c r="L26" t="s">
+        <v>24</v>
+      </c>
+      <c r="M26" t="s">
+        <v>26</v>
+      </c>
+      <c r="N26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27">
+        <v>2022</v>
+      </c>
+      <c r="E27">
+        <v>41.1</v>
+      </c>
+      <c r="F27">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="G27">
+        <v>102</v>
+      </c>
+      <c r="H27">
+        <v>97</v>
+      </c>
+      <c r="I27">
+        <v>107</v>
+      </c>
+      <c r="J27" s="1">
+        <v>120990</v>
+      </c>
+      <c r="K27" t="s">
+        <v>24</v>
+      </c>
+      <c r="L27" t="s">
+        <v>24</v>
+      </c>
+      <c r="M27" t="s">
+        <v>26</v>
+      </c>
+      <c r="N27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28">
+        <v>2022</v>
+      </c>
+      <c r="E28">
+        <v>41</v>
+      </c>
+      <c r="F28">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="G28">
+        <v>29</v>
+      </c>
+      <c r="H28">
+        <v>33</v>
+      </c>
+      <c r="I28">
+        <v>27</v>
+      </c>
+      <c r="J28" s="1">
+        <v>32735</v>
+      </c>
+      <c r="K28" t="s">
+        <v>29</v>
+      </c>
+      <c r="L28">
+        <v>4</v>
+      </c>
+      <c r="M28" t="s">
+        <v>26</v>
+      </c>
+      <c r="N28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29">
+        <v>2022</v>
+      </c>
+      <c r="E29">
+        <v>42.5</v>
+      </c>
+      <c r="F29">
+        <v>40.9</v>
+      </c>
+      <c r="G29">
+        <v>14</v>
+      </c>
+      <c r="H29">
+        <v>17</v>
+      </c>
+      <c r="I29">
+        <v>13</v>
+      </c>
+      <c r="J29" s="1">
+        <v>63830</v>
+      </c>
+      <c r="K29" t="s">
+        <v>29</v>
+      </c>
+      <c r="L29">
+        <v>8</v>
+      </c>
+      <c r="M29" t="s">
+        <v>26</v>
+      </c>
+      <c r="N29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30">
+        <v>2022</v>
+      </c>
+      <c r="E30">
+        <v>41.7</v>
+      </c>
+      <c r="F30">
+        <v>37.6</v>
+      </c>
+      <c r="G30">
+        <v>19</v>
+      </c>
+      <c r="H30">
+        <v>23</v>
+      </c>
+      <c r="I30">
+        <v>17</v>
+      </c>
+      <c r="J30" s="1">
+        <v>45855</v>
+      </c>
+      <c r="K30" t="s">
+        <v>29</v>
+      </c>
+      <c r="L30">
+        <v>6</v>
+      </c>
+      <c r="M30" t="s">
+        <v>26</v>
+      </c>
+      <c r="N30" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
relative paths to images
</commit_message>
<xml_diff>
--- a/Specs.xlsx
+++ b/Specs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gduncan\Downloads\vroom_vroom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F37FC1-ADA8-4182-ABFC-32CF344E4FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB6800A-A94F-41AB-A5F5-1A638C052B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A311B30-B3A1-4A32-B3E5-E04E58484C82}"/>
   </bookViews>
@@ -143,30 +143,6 @@
     <t>Image</t>
   </si>
   <si>
-    <t>C:\Users\gduncan\Downloads\vroom_vroom\images\Accord.jpg</t>
-  </si>
-  <si>
-    <t>C:\Users\gduncan\Downloads\vroom_vroom\images\CRV.jpg</t>
-  </si>
-  <si>
-    <t>C:\Users\gduncan\Downloads\vroom_vroom\images\Highlander.jpg</t>
-  </si>
-  <si>
-    <t>C:\Users\gduncan\Downloads\vroom_vroom\images\ModelY.jpg</t>
-  </si>
-  <si>
-    <t>C:\Users\gduncan\Downloads\vroom_vroom\images\QX60.jpg</t>
-  </si>
-  <si>
-    <t>C:\Users\gduncan\Downloads\vroom_vroom\images\RX350.jpg</t>
-  </si>
-  <si>
-    <t>C:\Users\gduncan\Downloads\vroom_vroom\images\Lyriq.jpg</t>
-  </si>
-  <si>
-    <t>C:\Users\gduncan\Downloads\vroom_vroom\images\Pilot.jpg</t>
-  </si>
-  <si>
     <t>Nissan</t>
   </si>
   <si>
@@ -264,6 +240,30 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>.\images\Accord.jpg</t>
+  </si>
+  <si>
+    <t>.\images\CRV.jpg</t>
+  </si>
+  <si>
+    <t>.\images\Highlander.jpg</t>
+  </si>
+  <si>
+    <t>.\images\ModelY.jpg</t>
+  </si>
+  <si>
+    <t>.\images\QX60.jpg</t>
+  </si>
+  <si>
+    <t>.\images\Lyriq.jpg</t>
+  </si>
+  <si>
+    <t>.\images\Pilot.jpg</t>
+  </si>
+  <si>
+    <t>.\images\RX350.jpg</t>
   </si>
 </sst>
 </file>
@@ -618,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB2CE35-0282-4446-A502-23F50F608244}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -731,7 +731,7 @@
         <v>33</v>
       </c>
       <c r="O2" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -778,7 +778,7 @@
         <v>33</v>
       </c>
       <c r="O3" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -825,7 +825,7 @@
         <v>33</v>
       </c>
       <c r="O4" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -872,7 +872,7 @@
         <v>33</v>
       </c>
       <c r="O5" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -919,7 +919,7 @@
         <v>33</v>
       </c>
       <c r="O6" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -966,7 +966,7 @@
         <v>33</v>
       </c>
       <c r="O7" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -1013,7 +1013,7 @@
         <v>33</v>
       </c>
       <c r="O8" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -1060,7 +1060,7 @@
         <v>33</v>
       </c>
       <c r="O9" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -1068,10 +1068,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D10">
         <v>2023</v>
@@ -1104,7 +1104,7 @@
         <v>26</v>
       </c>
       <c r="N10" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -1112,10 +1112,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D11">
         <v>2022</v>
@@ -1148,7 +1148,7 @@
         <v>26</v>
       </c>
       <c r="N11" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -1156,10 +1156,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D12">
         <v>2022</v>
@@ -1192,7 +1192,7 @@
         <v>26</v>
       </c>
       <c r="N12" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -1200,10 +1200,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D13">
         <v>2022</v>
@@ -1236,7 +1236,7 @@
         <v>26</v>
       </c>
       <c r="N13" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -1244,10 +1244,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D14">
         <v>2022</v>
@@ -1280,7 +1280,7 @@
         <v>26</v>
       </c>
       <c r="N14" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -1288,10 +1288,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D15">
         <v>2022</v>
@@ -1324,7 +1324,7 @@
         <v>26</v>
       </c>
       <c r="N15" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -1335,7 +1335,7 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D16">
         <v>2022</v>
@@ -1368,7 +1368,7 @@
         <v>28</v>
       </c>
       <c r="N16" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
@@ -1376,10 +1376,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D17">
         <v>2022</v>
@@ -1412,7 +1412,7 @@
         <v>26</v>
       </c>
       <c r="N17" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
@@ -1420,10 +1420,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D18">
         <v>2022</v>
@@ -1456,7 +1456,7 @@
         <v>26</v>
       </c>
       <c r="N18" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
@@ -1464,10 +1464,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D19">
         <v>2022</v>
@@ -1500,7 +1500,7 @@
         <v>26</v>
       </c>
       <c r="N19" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
@@ -1508,10 +1508,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D20">
         <v>2022</v>
@@ -1544,7 +1544,7 @@
         <v>26</v>
       </c>
       <c r="N20" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
@@ -1552,10 +1552,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D21">
         <v>2022</v>
@@ -1588,7 +1588,7 @@
         <v>26</v>
       </c>
       <c r="N21" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
@@ -1596,10 +1596,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D22">
         <v>2022</v>
@@ -1632,7 +1632,7 @@
         <v>26</v>
       </c>
       <c r="N22" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
@@ -1640,10 +1640,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D23">
         <v>2022</v>
@@ -1676,7 +1676,7 @@
         <v>26</v>
       </c>
       <c r="N23" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
@@ -1684,10 +1684,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D24">
         <v>2022</v>
@@ -1720,7 +1720,7 @@
         <v>26</v>
       </c>
       <c r="N24" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
@@ -1731,7 +1731,7 @@
         <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D25">
         <v>2022</v>
@@ -1764,7 +1764,7 @@
         <v>26</v>
       </c>
       <c r="N25" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
@@ -1775,7 +1775,7 @@
         <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D26">
         <v>2022</v>
@@ -1808,7 +1808,7 @@
         <v>26</v>
       </c>
       <c r="N26" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
@@ -1819,7 +1819,7 @@
         <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D27">
         <v>2022</v>
@@ -1852,7 +1852,7 @@
         <v>26</v>
       </c>
       <c r="N27" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
@@ -1863,7 +1863,7 @@
         <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D28">
         <v>2022</v>
@@ -1896,7 +1896,7 @@
         <v>26</v>
       </c>
       <c r="N28" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
@@ -1907,7 +1907,7 @@
         <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D29">
         <v>2022</v>
@@ -1940,7 +1940,7 @@
         <v>26</v>
       </c>
       <c r="N29" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
@@ -1948,10 +1948,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C30" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D30">
         <v>2022</v>
@@ -1984,7 +1984,7 @@
         <v>26</v>
       </c>
       <c r="N30" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>